<commit_message>
Correc Borneras - revision nicolas
</commit_message>
<xml_diff>
--- a/Lista_elementos_PCB.xlsx
+++ b/Lista_elementos_PCB.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PCB_ESP_CON_USB\Nilm_project_V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PCB_ESP_USB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDFB52-F046-4E2D-B89A-044D8B359A09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1808A51D-D188-4E6F-8263-3F239ECB1E39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C569EA13-9E1A-4641-A49C-E2C94A5316D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C569EA13-9E1A-4641-A49C-E2C94A5316D6}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTA ELEMENTOS" sheetId="1" r:id="rId1"/>
+    <sheet name="COTIZACION_DIGIKEY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="126">
   <si>
     <t>CANTIDAD</t>
   </si>
@@ -198,6 +195,216 @@
   </si>
   <si>
     <t>CAPACITOR 0.01UF</t>
+  </si>
+  <si>
+    <t>COTIZACIÓN ELEMENTOS PROJECT NILM-UIS EN DIGIKEY</t>
+  </si>
+  <si>
+    <t>P / UNIDAD</t>
+  </si>
+  <si>
+    <t>P / TOTAL</t>
+  </si>
+  <si>
+    <t>PART NUMBER</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32</t>
+  </si>
+  <si>
+    <t>1904-1010-1-ND</t>
+  </si>
+  <si>
+    <t>REG 3.3V - LM1117</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/espressif-systems/ESP32-WROOM-32/1904-1010-1-ND/8544305</t>
+  </si>
+  <si>
+    <t>LM1117MPX-3.3/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/LM1117MPX-3-3-NOPB/LM1117MPX-3-3-NOPBCT-ND/1010516</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE B3U-1000P</t>
+  </si>
+  <si>
+    <t>SW1020CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/omron-electronics-inc-emc-div/B3U-1000P/SW1020CT-ND/1534357</t>
+  </si>
+  <si>
+    <t>SENSOR TEMP - TMP275AIDR</t>
+  </si>
+  <si>
+    <t>296-39296-1-ND</t>
+  </si>
+  <si>
+    <t>INA821ID</t>
+  </si>
+  <si>
+    <t>8 - SOIC</t>
+  </si>
+  <si>
+    <t>296-53404-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/TMP275AIDR/296-39296-1-ND/5143286/?itemSeq=319271916</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/INA821ID/296-53404-ND/9858339</t>
+  </si>
+  <si>
+    <t>CP2102-GM</t>
+  </si>
+  <si>
+    <t>QFN - 28</t>
+  </si>
+  <si>
+    <t>336-5890-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/silicon-labs/CP2102N-A02-GQFN28R/336-5890-1-ND/9863483</t>
+  </si>
+  <si>
+    <t>TPD2S017DBVR</t>
+  </si>
+  <si>
+    <t>SOT - 23</t>
+  </si>
+  <si>
+    <t>296-25216-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/TPD2S017DBVR/296-25216-1-ND/2172703/?itemSeq=317171693</t>
+  </si>
+  <si>
+    <t>TRANS NPN - MMSS8050-L-TP</t>
+  </si>
+  <si>
+    <t>MMSS8050-L-TPMSCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/MMSS8050-L-TP/MMSS8050-L-TPMSCT-ND/2827203/?itemSeq=324663815</t>
+  </si>
+  <si>
+    <t>MICRO USB B - 10118192-001LF</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/10118192-0001LF/609-4613-1-ND/2785378/?itemSeq=317169616</t>
+  </si>
+  <si>
+    <t>SMD - 0805</t>
+  </si>
+  <si>
+    <t>475-1410-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/LG+R971-KN-1/475-1410-1-ND/1802598/?itemSeq=317171616</t>
+  </si>
+  <si>
+    <t>475-1415-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/LH+R974-LP-1/475-1415-1-ND/1802604/?itemSeq=317171622</t>
+  </si>
+  <si>
+    <t>490-13982-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/GRM31CR60J107KE39L/490-13982-1-ND/6155812/?itemSeq=317169822</t>
+  </si>
+  <si>
+    <t>CAPACITOR 100 UF</t>
+  </si>
+  <si>
+    <t>CAPACITOR 0.1 UF</t>
+  </si>
+  <si>
+    <t>399-17616-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/C0805C103J5RAC7210/399-17616-1-ND/8572616/?itemSeq=325112023</t>
+  </si>
+  <si>
+    <t>CAPACITOR 0.01 UF</t>
+  </si>
+  <si>
+    <t>399-1171-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0805C104J5RACTU/399-1171-1-ND/411446</t>
+  </si>
+  <si>
+    <t>CAPACITOR 1 UF</t>
+  </si>
+  <si>
+    <t>311-3498-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/CC0805JKX7R9BB105/311-3498-1-ND/7164519</t>
+  </si>
+  <si>
+    <t>CAPACITOR 4.7 UF</t>
+  </si>
+  <si>
+    <t>399-15708-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0805C475J8RACAUTO/399-15708-1-ND/7427588</t>
+  </si>
+  <si>
+    <t>CAPACITOR 10 UF</t>
+  </si>
+  <si>
+    <t>399-15693-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0805C106J8RACAUTO/399-15693-1-ND/7427573</t>
+  </si>
+  <si>
+    <t>A129761CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/CRGCQ0805F10K/A129761CT-ND/8577593/?itemSeq=317170571</t>
+  </si>
+  <si>
+    <t>RESISTENCIA 5K</t>
+  </si>
+  <si>
+    <t>541-4321-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/CRCW08055K00FKTA/541-4321-1-ND/8565934/?itemSeq=319272543</t>
+  </si>
+  <si>
+    <t>A126337CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/CRG0805F12K/A126337CT-ND/7603392/?itemSeq=317170622</t>
+  </si>
+  <si>
+    <t>P20936CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ERJ-PB6B1004V/P20936CT-ND/6215191/?itemSeq=325112308</t>
+  </si>
+  <si>
+    <t>RESISTENCIA 25K (24,7K)</t>
+  </si>
+  <si>
+    <t>A121556CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-passive-product/CPF0805B25KE1/A121556CT-ND/5246518</t>
   </si>
 </sst>
 </file>
@@ -208,7 +415,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +442,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,11 +528,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,14 +580,22 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -687,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9F9874-75CC-47D4-A49B-F62B545DB624}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,18 +927,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1348,4 +1572,626 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA253C7F-76B5-472D-8E52-EB4D43CF2177}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3">
+        <v>3.8</v>
+      </c>
+      <c r="F3">
+        <f>E3*A3</f>
+        <v>3.8</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F26" si="0">E4*A4</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5">
+        <v>0.98</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>3.35</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3.35</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>6.19</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>6.19</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8">
+        <v>1.4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
+        <v>0.61</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10">
+        <v>0.18</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11">
+        <v>0.43</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12">
+        <v>0.26</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13">
+        <v>0.26</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14">
+        <v>0.76</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15">
+        <v>0.19</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>0.11</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17">
+        <v>0.33</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18">
+        <v>0.61</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19">
+        <v>0.83</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1.66</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22">
+        <v>0.1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23">
+        <v>0.36</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24">
+        <v>0.65</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{D2267DC0-AD2B-47AA-AF55-A223964E093D}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{2165ABB4-AB49-4BE4-8EB4-C8347789B221}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{5DD75587-9181-4900-B109-CD6B3DA6507F}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{1EC30833-7C7E-4507-B5F1-235456D1E1EB}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{952BA3F0-F045-4114-A287-DD3B86F94C93}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{EAE89E54-F958-40D7-9A37-E411D0EF8C1B}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{8C7DD61F-5DAA-45DA-BB0E-07E8AE4F0AE1}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{73F4DC57-3DD2-4B8D-A991-2381D5E81145}"/>
+    <hyperlink ref="G11" r:id="rId9" xr:uid="{DD752C59-6FD1-40A2-B702-D2C1B63B1094}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{56F43060-EC90-4B3A-873C-F4748143C9A2}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{7B81D068-D73A-4F4F-A801-1CB33329397E}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{4B8286E9-4E0A-41FC-A3BC-C5F2DFD2DB22}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{6B0E7E7E-3D23-417B-91BB-316F04B44E4E}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{039670BA-BED2-4D2E-BC86-20C543408B1D}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{581074DF-BE6D-424E-8DBC-38C5C9744DBE}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{4EEFFCF1-9357-4A30-9FF3-763C2C06BE7C}"/>
+    <hyperlink ref="G20" r:id="rId17" xr:uid="{A7F53AC4-A57D-4920-9573-DC2C1F030494}"/>
+    <hyperlink ref="G21" r:id="rId18" xr:uid="{B15B9AA7-4FFF-4A6B-B407-13D135FC1584}"/>
+    <hyperlink ref="G22" r:id="rId19" xr:uid="{068CCF8A-FE42-4BA7-8ADF-3A20B438EF06}"/>
+    <hyperlink ref="G23" r:id="rId20" xr:uid="{77292D12-E813-4458-B53B-3475CC93D37B}"/>
+    <hyperlink ref="G24" r:id="rId21" xr:uid="{531BA87B-65DF-4110-8382-E8E0BA7B03F3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lista elementos terminada - revision nicolas
</commit_message>
<xml_diff>
--- a/Lista_elementos_PCB.xlsx
+++ b/Lista_elementos_PCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PCB_ESP_USB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1808A51D-D188-4E6F-8263-3F239ECB1E39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B436162-3F72-4978-A525-359F5061A515}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C569EA13-9E1A-4641-A49C-E2C94A5316D6}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="COTIZACION_DIGIKEY" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="151">
   <si>
     <t>CANTIDAD</t>
   </si>
@@ -405,6 +404,81 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/te-connectivity-passive-product/CPF0805B25KE1/A121556CT-ND/5246518</t>
+  </si>
+  <si>
+    <t>BORNERAS 2 POSICIONES</t>
+  </si>
+  <si>
+    <t>THROUGH HOLE</t>
+  </si>
+  <si>
+    <t>277-6405-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/phoenix-contact/1935776/277-6405-ND/2513905</t>
+  </si>
+  <si>
+    <t>BORNERAS 3 POSICIONES</t>
+  </si>
+  <si>
+    <t>277-6072-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/phoenix-contact/1935789/277-6072-ND/2513906</t>
+  </si>
+  <si>
+    <t>PIN HEADER X2 POSICIONES</t>
+  </si>
+  <si>
+    <t>732-5315-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/w%C3%BCrth-elektronik/61300211121/732-5315-ND/4846823</t>
+  </si>
+  <si>
+    <t>JUMPER CONECTOR</t>
+  </si>
+  <si>
+    <t>S9337-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/QPC02SXGN-RC/S9337-ND/2618262</t>
+  </si>
+  <si>
+    <t>PIN HEADER X9 POSICIONES</t>
+  </si>
+  <si>
+    <t>732-5322-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/w%C3%BCrth-elektronik/61300911121/732-5322-ND/4846843</t>
+  </si>
+  <si>
+    <t>BULK</t>
+  </si>
+  <si>
+    <t>PIN HEADER X1 POSICIONES</t>
+  </si>
+  <si>
+    <t>609-3466-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/amphenol-icc-fci/68000-401HLF/609-3466-ND/2023286</t>
+  </si>
+  <si>
+    <t>ENVIO USA</t>
+  </si>
+  <si>
+    <t>ENVIO USA-COL</t>
+  </si>
+  <si>
+    <t>TOTAL (USD)</t>
+  </si>
+  <si>
+    <t>TOTAL (COP)</t>
+  </si>
+  <si>
+    <t>DIVISA DÓLAR</t>
   </si>
 </sst>
 </file>
@@ -455,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,8 +566,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -527,13 +607,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -580,17 +669,19 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -927,18 +1018,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1576,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA253C7F-76B5-472D-8E52-EB4D43CF2177}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,585 +1679,769 @@
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="113" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>3.8</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <f>E3*A3</f>
         <v>3.8</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="22" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F26" si="0">E4*A4</f>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F30" si="0">E4*A4</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="22" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>0.98</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>1.96</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>3.35</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>3.35</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>6.19</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>6.19</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="22" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>1.4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>0.61</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>0.61</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="22" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>0.18</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="22" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>0.43</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="22" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>0.26</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>0.26</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>0.76</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="4">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>0.19</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="5">
         <f t="shared" si="0"/>
         <v>1.1400000000000001</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="22" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="4">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>0.11</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="22" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="4">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>0.33</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="5">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="22" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>0.61</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="5">
         <f t="shared" si="0"/>
         <v>0.61</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="22" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="4">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>0.83</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="5">
         <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="22" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="4">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>0.1</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="22" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="4">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
         <v>0.42000000000000004</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="22" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="4">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>0.1</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="5">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="22" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>0.36</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="22" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>0.65</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="5">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="22" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A25" s="4">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>4</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.41</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="0"/>
+        <v>1.64</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.11</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="5">
+        <f>SUM(F3:F30)</f>
+        <v>30.760000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="26">
+        <v>3800</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="25">
+        <f>SUM(F32:F34)</f>
+        <v>64.760000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="25">
+        <f>F35*C35</f>
+        <v>246088.00000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{D2267DC0-AD2B-47AA-AF55-A223964E093D}"/>
@@ -2190,8 +2465,14 @@
     <hyperlink ref="G22" r:id="rId19" xr:uid="{068CCF8A-FE42-4BA7-8ADF-3A20B438EF06}"/>
     <hyperlink ref="G23" r:id="rId20" xr:uid="{77292D12-E813-4458-B53B-3475CC93D37B}"/>
     <hyperlink ref="G24" r:id="rId21" xr:uid="{531BA87B-65DF-4110-8382-E8E0BA7B03F3}"/>
+    <hyperlink ref="G25" r:id="rId22" xr:uid="{A776219D-57CF-4D40-926D-6C633FEE8781}"/>
+    <hyperlink ref="G26" r:id="rId23" xr:uid="{9202890C-0FC4-41D0-BBFA-DCE18DBFD7B8}"/>
+    <hyperlink ref="G27" r:id="rId24" xr:uid="{597D33DB-02B2-4EBD-8530-5BE072DA552E}"/>
+    <hyperlink ref="G28" r:id="rId25" xr:uid="{17BBD72D-59D7-4022-93FF-61E3A115C343}"/>
+    <hyperlink ref="G29" r:id="rId26" xr:uid="{2812BA70-76F4-464B-8B42-408CE2DFD3E2}"/>
+    <hyperlink ref="G30" r:id="rId27" xr:uid="{374E39AE-8C8C-43E4-B5E5-B8DEFD9BFFDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>